<commit_message>
dont L2O, ScaleL2O, UNet, UNetL2O
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62c898fd010bc8e6/Desktop/UNetL2O/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="13_ncr:1_{BA8AB4BA-576C-404C-B542-3703D65D273C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E90CD07C-C88F-4A62-B834-91433A174B8D}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{BA8AB4BA-576C-404C-B542-3703D65D273C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B781BCB3-39FF-41C2-97F2-F15DFCE8126A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1458,7 +1458,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1845,10 +1845,10 @@
         <v>0</v>
       </c>
       <c r="E18" s="18">
-        <v>3.3000000000000002E-2</v>
+        <v>0.04</v>
       </c>
       <c r="F18" s="24">
-        <v>5.0999999999999997E-2</v>
+        <v>0.05</v>
       </c>
       <c r="G18" s="13">
         <v>485780</v>

</xml_diff>